<commit_message>
add Minimum Moves to Reach Target Score
</commit_message>
<xml_diff>
--- a/experimaentResult.xlsx
+++ b/experimaentResult.xlsx
@@ -12,7 +12,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9132"/>
   </bookViews>
   <sheets>
-    <sheet name="clz" sheetId="1" r:id="rId1"/>
+    <sheet name="cz" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="33">
   <si>
     <t>0x00000000</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -115,6 +115,46 @@
   </si>
   <si>
     <t>-2147483648/1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>x</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">bug </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MinimumMovestoReachTargetScore</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>target/maxMoves</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>157561568/12</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>565868992/3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>19/2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>565868992/41</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>12566397/100</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10/2</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -199,7 +239,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -259,13 +299,33 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -287,6 +347,9 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -296,7 +359,10 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -314,6 +380,66 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="圖片 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="14775180" y="3291840"/>
+          <a:ext cx="14782800" cy="1859280"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -579,10 +705,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="D3" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
@@ -867,15 +993,15 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="9"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="10"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
@@ -938,7 +1064,9 @@
       <c r="F22" s="2">
         <v>1.4</v>
       </c>
-      <c r="G22" s="2"/>
+      <c r="G22" s="2" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
@@ -977,29 +1105,201 @@
       <c r="E24" s="2">
         <v>0</v>
       </c>
-      <c r="F24" s="10">
+      <c r="F24" s="7">
         <v>0</v>
       </c>
-      <c r="G24" s="10"/>
+      <c r="G24" s="7" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="7" t="s">
+      <c r="A25" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B25" s="8"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="8"/>
-      <c r="F25" s="8"/>
-      <c r="G25" s="9"/>
+      <c r="B25" s="9"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="10"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B31" s="12"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G32" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B33" s="9"/>
+      <c r="C33" s="9"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
+      <c r="G33" s="10"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B34" s="2">
+        <v>401</v>
+      </c>
+      <c r="C34" s="2">
+        <v>1054</v>
+      </c>
+      <c r="D34" s="2">
+        <v>119</v>
+      </c>
+      <c r="E34" s="2">
+        <v>193</v>
+      </c>
+      <c r="F34" s="2">
+        <v>1340</v>
+      </c>
+      <c r="G34" s="2">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A35" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B35" s="2">
+        <v>271</v>
+      </c>
+      <c r="C35" s="2">
+        <v>712</v>
+      </c>
+      <c r="D35" s="2">
+        <v>81</v>
+      </c>
+      <c r="E35" s="2">
+        <v>129</v>
+      </c>
+      <c r="F35" s="2">
+        <v>900</v>
+      </c>
+      <c r="G35" s="2">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A36" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B36" s="2">
+        <v>1.48</v>
+      </c>
+      <c r="C36" s="2">
+        <v>1.48</v>
+      </c>
+      <c r="D36" s="2">
+        <v>1.47</v>
+      </c>
+      <c r="E36" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="F36" s="2">
+        <v>1.49</v>
+      </c>
+      <c r="G36" s="2">
+        <v>1.49</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A37" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B37" s="2">
+        <v>0.67600000000000005</v>
+      </c>
+      <c r="C37" s="2">
+        <v>0.67600000000000005</v>
+      </c>
+      <c r="D37" s="2">
+        <v>0.68100000000000005</v>
+      </c>
+      <c r="E37" s="2">
+        <v>0.66800000000000004</v>
+      </c>
+      <c r="F37" s="2">
+        <v>0.67200000000000004</v>
+      </c>
+      <c r="G37" s="2">
+        <v>0.67100000000000004</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A38" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B38" s="2">
+        <v>38482</v>
+      </c>
+      <c r="C38" s="2">
+        <v>42</v>
+      </c>
+      <c r="D38" s="2">
+        <v>7073626</v>
+      </c>
+      <c r="E38" s="2">
+        <v>7</v>
+      </c>
+      <c r="F38" s="2">
+        <v>42</v>
+      </c>
+      <c r="G38" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A39" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B39" s="9"/>
+      <c r="C39" s="9"/>
+      <c r="D39" s="9"/>
+      <c r="E39" s="9"/>
+      <c r="F39" s="9"/>
+      <c r="G39" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="5">
     <mergeCell ref="A19:G19"/>
     <mergeCell ref="A25:G25"/>
+    <mergeCell ref="A33:G33"/>
+    <mergeCell ref="A39:G39"/>
+    <mergeCell ref="A31:B31"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>